<commit_message>
Finish tod adult norms, rerun grade for ORF in school-age sample
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/gea_sum-adult-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/gea_sum-adult-raw-ss-lookup-tabbed-age.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,151 +376,151 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>82</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>84</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>86</v>
@@ -544,153 +544,161 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>
@@ -701,7 +709,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -721,159 +729,159 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>84</v>
@@ -881,15 +889,15 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>87</v>
@@ -897,7 +905,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>89</v>
@@ -905,7 +913,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>91</v>
@@ -913,129 +921,137 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>
@@ -1046,7 +1062,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1066,175 +1082,175 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>88</v>
@@ -1242,7 +1258,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>90</v>
@@ -1250,15 +1266,15 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>93</v>
@@ -1266,7 +1282,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>95</v>
@@ -1274,7 +1290,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>97</v>
@@ -1282,7 +1298,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>99</v>
@@ -1290,7 +1306,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>101</v>
@@ -1298,89 +1314,97 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>
@@ -1391,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1411,321 +1435,329 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>
@@ -1736,7 +1768,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1756,311 +1788,311 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>130</v>
@@ -2068,9 +2100,17 @@
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>
@@ -2081,7 +2121,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2101,287 +2141,287 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>130</v>
@@ -2389,7 +2429,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>130</v>
@@ -2397,7 +2437,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>130</v>
@@ -2405,7 +2445,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>130</v>
@@ -2413,9 +2453,17 @@
     </row>
     <row r="41">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>130</v>
       </c>
     </row>

</xml_diff>